<commit_message>
projedeki eksiklikler giderildi, report eklendi
</commit_message>
<xml_diff>
--- a/src/test/java/Sonuc/TestSonuclari.xlsx
+++ b/src/test/java/Sonuc/TestSonuclari.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selçuk\IdeaProjects\Cucumber_Project1\src\test\java\Sonuc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9971DD-40DA-4654-8503-DCB59BBD04A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF828BA2-3047-46A8-8C3A-F090758B6A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="9">
   <si>
     <t>New Account Creation</t>
   </si>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A18:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,7 +458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -466,7 +466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -474,7 +474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -482,44 +482,428 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>6</v>
-      </c>
       <c r="B14" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>